<commit_message>
Fixes on Excel service
</commit_message>
<xml_diff>
--- a/api/src/Service/resources/components.xlsx
+++ b/api/src/Service/resources/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\environment-component\api\src\Service\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF839C8A-6325-4B24-90D9-F184D6D22AD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7D5C6C-C936-4258-9A90-DBBACBA7DA74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
+    <workbookView xWindow="3300" yWindow="165" windowWidth="21600" windowHeight="15435" activeTab="1" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
   </bookViews>
   <sheets>
     <sheet name="clusters" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>evc</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Een domein voor ROC experimenten</t>
+  </si>
+  <si>
+    <t>9-4-2020</t>
   </si>
 </sst>
 </file>
@@ -193,9 +196,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -546,10 +551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0233B350-72AF-4D84-A15D-5E384E813B54}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,9 +563,10 @@
     <col min="3" max="3" width="67.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -576,11 +582,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1">
+      <c r="F1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -593,11 +599,14 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -610,11 +619,11 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -627,11 +636,12 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -644,11 +654,12 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -661,11 +672,14 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -678,7 +692,7 @@
       <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -694,7 +708,7 @@
     <hyperlink ref="D6" r:id="rId8" xr:uid="{F7E95135-2938-42E0-8AF7-CA6E5A4EFEF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Excel for processencluster, temp performance fixes
</commit_message>
<xml_diff>
--- a/api/src/Service/resources/components.xlsx
+++ b/api/src/Service/resources/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\environment-component\api\src\Service\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC17AB64-E694-4ECE-B0E9-8C658DD1CA89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B49B97-6271-4825-805C-47AEA540B1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="97">
   <si>
     <t>evc</t>
   </si>
@@ -50,21 +50,6 @@
     <t>https://github.com/ConductionNL/environment-component/api/helm</t>
   </si>
   <si>
-    <t>uc</t>
-  </si>
-  <si>
-    <t>User Component</t>
-  </si>
-  <si>
-    <t>mrc</t>
-  </si>
-  <si>
-    <t>Medewerkercomponent</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/medewerkercatalogus/api/helm</t>
-  </si>
-  <si>
     <t>wrc</t>
   </si>
   <si>
@@ -101,21 +86,12 @@
     <t>https://github.com/ConductionNL/environment-component</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/user-component</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/medewerkercatalogus</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/webresourcecatalogus</t>
   </si>
   <si>
     <t>https://github.com/ConductionNL/digispoof-interface</t>
   </si>
   <si>
-    <t>9-4-2020</t>
-  </si>
-  <si>
     <t>cc</t>
   </si>
   <si>
@@ -128,9 +104,6 @@
     <t>https://github.com/ConductionNL/contactcatalogus/api/helm</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/user-component/api/helm</t>
-  </si>
-  <si>
     <t>irc</t>
   </si>
   <si>
@@ -143,51 +116,6 @@
     <t>https://github.com/ConductionNL/instemmingservice/api/helm</t>
   </si>
   <si>
-    <t>Agendacomponent</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/agendaservice</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/agendaservice/api/helm</t>
-  </si>
-  <si>
-    <t>pdc</t>
-  </si>
-  <si>
-    <t>productenendienstencatalogus</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/productenendienstencatalogus</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/productenendienstencatalogus/api/helm</t>
-  </si>
-  <si>
-    <t>orc</t>
-  </si>
-  <si>
-    <t>orderregistratiecomponent</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/orderregistratiecomponent</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/orderregistratiecomponent/api/helm</t>
-  </si>
-  <si>
-    <t>lc</t>
-  </si>
-  <si>
-    <t>locatiecomponent</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/locatiecatalogus</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/locatiecatalogus/api/helm</t>
-  </si>
-  <si>
     <t>vtc</t>
   </si>
   <si>
@@ -212,18 +140,6 @@
     <t>https://github.com/ConductionNL/verzoekregistratiecomponent/api/helm</t>
   </si>
   <si>
-    <t>bc</t>
-  </si>
-  <si>
-    <t>betaalcomponent</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/betaalservice</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/betaalservice/api/helm</t>
-  </si>
-  <si>
     <t>brp</t>
   </si>
   <si>
@@ -236,102 +152,6 @@
     <t>https://github.com/ConductionNL/brpservice/api/helm</t>
   </si>
   <si>
-    <t>bs</t>
-  </si>
-  <si>
-    <t>berichtservice</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/berichtservice</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/berichtservice/api/helm</t>
-  </si>
-  <si>
-    <t>stuf</t>
-  </si>
-  <si>
-    <t>stufservice</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/stufservice</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/stufservice/api/helm</t>
-  </si>
-  <si>
-    <t>irc-ui</t>
-  </si>
-  <si>
-    <t>instemming-ui</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/instemming-interface</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/instemming-interface/api/helm</t>
-  </si>
-  <si>
-    <t>hpui</t>
-  </si>
-  <si>
-    <t>huwelijksplanner-ui</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/huwelijksplanner-ui</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/huwelijksplanner-ui/api/helm</t>
-  </si>
-  <si>
-    <t>bbz-ui</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/corona-interface</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/corona-interface/api/helm</t>
-  </si>
-  <si>
-    <t>bbz ui</t>
-  </si>
-  <si>
-    <t>db</t>
-  </si>
-  <si>
-    <t>dashboard</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/commonground-dashboard</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/commonground-dashboard/api/helm</t>
-  </si>
-  <si>
-    <t>bzk-ui</t>
-  </si>
-  <si>
-    <t>developer conduction</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/bzk-mock</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/bzk-mock/api/helm</t>
-  </si>
-  <si>
-    <t>conweb</t>
-  </si>
-  <si>
-    <t>conduction website</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/conductionwebsite</t>
-  </si>
-  <si>
-    <t>https://github.com/ConductionNL/conductionwebsite/api/helm</t>
-  </si>
-  <si>
     <t>The environment excel file</t>
   </si>
   <si>
@@ -437,9 +257,6 @@
     <t>no (defaults to FALSE)</t>
   </si>
   <si>
-    <t>arc</t>
-  </si>
-  <si>
     <t>huwelijksplanner</t>
   </si>
   <si>
@@ -450,6 +267,66 @@
   </si>
   <si>
     <t>https://huwelijksplanner.online</t>
+  </si>
+  <si>
+    <t>processen</t>
+  </si>
+  <si>
+    <t>het processen cluster</t>
+  </si>
+  <si>
+    <t>het processen domein</t>
+  </si>
+  <si>
+    <t>https://processen.zaakonline.nl</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>Adresservice</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/adresservice</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/adresservice/api/helm</t>
+  </si>
+  <si>
+    <t>ltc</t>
+  </si>
+  <si>
+    <t>Landelijketabellencatalogus</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/landelijketabellencatalogus</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/landelijketabellencatalogus/api/helm</t>
+  </si>
+  <si>
+    <t>prc</t>
+  </si>
+  <si>
+    <t>procesregistratiecomponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/procesregistratiecomponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/procesregistratiecomponent/api/helm</t>
+  </si>
+  <si>
+    <t>ptc</t>
+  </si>
+  <si>
+    <t>procestypecatalogus</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/procestypecatalogus</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/procestypecatalogus/api/helm</t>
   </si>
 </sst>
 </file>
@@ -891,12 +768,12 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="47.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -910,7 +787,7 @@
     </row>
     <row r="4" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -924,203 +801,203 @@
     </row>
     <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>115</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>121</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>126</v>
+        <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="H22" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1136,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D686253-1BB3-4847-8D4A-74F469441A53}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,20 +1027,31 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="1"/>
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
@@ -1186,6 +1074,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" xr:uid="{237A0970-0A96-4FCB-B918-C04A244A79F5}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{C3E36D05-41DF-4034-BE99-7576B7E24291}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1208,30 +1097,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1241,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0233B350-72AF-4D84-A15D-5E384E813B54}">
-  <dimension ref="A1:XFD24"/>
+  <dimension ref="A1:XFD27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,83 +1147,74 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="F1" t="b">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1347,7 +1227,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -1355,407 +1235,230 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
+        <v>87</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="XFD24" s="1"/>
     </row>
+    <row r="25" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="4:7 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F27">
+    <sortCondition ref="A1"/>
+  </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D18" r:id="rId1" xr:uid="{19D77A23-42EE-4254-8245-A81D77BFF7C7}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{6DB4D0C8-8136-4767-8BB6-9EAFDDDC6960}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{C40D44EA-D742-448C-9AEC-1F4732849AC9}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{3FD9B41C-CA07-4E4B-ADC0-B0179A8307EE}"/>
-    <hyperlink ref="D1" r:id="rId5" xr:uid="{F7E95135-2938-42E0-8AF7-CA6E5A4EFEF3}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{8D635CA0-58C6-4BAC-ADD8-803599AD66DE}"/>
-    <hyperlink ref="E3" r:id="rId7" xr:uid="{2834821C-30B7-4BAB-A1CF-5FA292E134C3}"/>
-    <hyperlink ref="E2" r:id="rId8" xr:uid="{216588E6-C76E-4980-B24A-36F84C01C192}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{41FE42E3-3745-4DB9-BAF7-CCAA19F6AE02}"/>
-    <hyperlink ref="E4" r:id="rId10" xr:uid="{7CED1F56-7CEE-4740-AE25-A1F5ACD1F0BA}"/>
-    <hyperlink ref="D6" r:id="rId11" xr:uid="{AC764AAA-B58C-4954-B029-5E294B592161}"/>
-    <hyperlink ref="E6" r:id="rId12" xr:uid="{46B7C202-6861-486C-B246-B4373C323B1A}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{6BEE194D-A489-4F62-B948-8B16F9FF5F11}"/>
-    <hyperlink ref="E8" r:id="rId14" xr:uid="{2F754EA3-D2C4-4DD4-8814-7222312F8F43}"/>
-    <hyperlink ref="D9" r:id="rId15" xr:uid="{141198DF-20C7-4B92-9BCD-AB74D27BF65D}"/>
-    <hyperlink ref="E9" r:id="rId16" xr:uid="{0D5F5E6D-0D6F-429D-9A0C-D67EC7CBD986}"/>
-    <hyperlink ref="D10" r:id="rId17" xr:uid="{F11678A0-3378-4310-B596-597F2BEBC93E}"/>
-    <hyperlink ref="E10" r:id="rId18" xr:uid="{97E05BAB-7404-43F8-8F44-02D4409EE054}"/>
-    <hyperlink ref="D11" r:id="rId19" xr:uid="{CDE1DE1F-C04F-4955-8CA7-40DDCE2A7869}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{B7C41ED0-0748-466D-A777-87C0221011B3}"/>
-    <hyperlink ref="D12" r:id="rId21" xr:uid="{7EFE02F7-EA53-438F-8D7B-1EE7A8F2ACCF}"/>
-    <hyperlink ref="E12" r:id="rId22" xr:uid="{8DCB265B-8E3C-4980-ABC7-8A6393434105}"/>
-    <hyperlink ref="D13" r:id="rId23" xr:uid="{C0D05A4F-6CD6-4877-A4E9-ADE0BDD030E8}"/>
-    <hyperlink ref="E13" r:id="rId24" xr:uid="{9E4C2216-4B71-4B1E-B43D-1054E19CCF38}"/>
-    <hyperlink ref="D14" r:id="rId25" xr:uid="{36AA91A0-C9BC-4B14-A2ED-34EDE64D808F}"/>
-    <hyperlink ref="E14" r:id="rId26" xr:uid="{7F2186DB-5F0A-478D-8ABA-18A632F4AFA9}"/>
-    <hyperlink ref="D15" r:id="rId27" xr:uid="{677457FC-2A7F-458E-8520-A3608E770BD0}"/>
-    <hyperlink ref="E15" r:id="rId28" xr:uid="{B0DA4668-9A77-414A-8D9C-BE2AF37F4004}"/>
-    <hyperlink ref="E16" r:id="rId29" xr:uid="{04B35525-5C64-4A32-85FC-D5A412CE50BE}"/>
-    <hyperlink ref="D16" r:id="rId30" xr:uid="{520950D5-5F78-405A-8D34-933ADD02C75A}"/>
-    <hyperlink ref="D19" r:id="rId31" xr:uid="{4E1C3029-B966-4AFC-969F-5012C6A4D8C6}"/>
-    <hyperlink ref="E19" r:id="rId32" xr:uid="{9BF3B3A1-96CB-4148-AE02-5056D4E200B3}"/>
-    <hyperlink ref="D20" r:id="rId33" xr:uid="{66758EAE-75EA-44AA-9DF4-688290D5778A}"/>
-    <hyperlink ref="E20" r:id="rId34" xr:uid="{0A05031E-03E0-4A3E-8EE6-23150FC73ED4}"/>
-    <hyperlink ref="E21" r:id="rId35" xr:uid="{48139D65-5882-4852-8315-6AC52C7C4889}"/>
-    <hyperlink ref="D17" r:id="rId36" xr:uid="{F3967BE9-349C-465E-AABA-888AE310A716}"/>
-    <hyperlink ref="E17" r:id="rId37" xr:uid="{D4DE7FA9-523B-4683-B13A-38C1004F34CE}"/>
-    <hyperlink ref="D22" r:id="rId38" xr:uid="{1339A50A-19D6-4E2D-97B8-8A94407EB924}"/>
-    <hyperlink ref="E22" r:id="rId39" xr:uid="{86286767-67F3-43F7-96E0-F949BFD50658}"/>
-    <hyperlink ref="D23" r:id="rId40" xr:uid="{2ADFB7BD-711E-4EF8-A942-9A466D75DCE3}"/>
-    <hyperlink ref="E23" r:id="rId41" xr:uid="{7FD1FD3F-CF94-4FEE-BA82-467B3BCF9768}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{19D77A23-42EE-4254-8245-A81D77BFF7C7}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{B2C0F910-C780-487C-8626-37471E064F3C}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{F6B800C5-0340-4308-BF0D-EEE018D29771}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{19999326-0F9D-47EC-8344-5D251838B379}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{99226445-1AF8-421E-BE28-28BCEA591327}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{7AAD05D6-0D94-46F6-A622-9ADE928F6D82}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{BE91BA4C-1FBD-4F66-B42D-1AB0CB92D216}"/>
+    <hyperlink ref="E1" r:id="rId8" xr:uid="{3A2E2778-4B07-40A7-84C1-331EBA3BFF80}"/>
+    <hyperlink ref="D1" r:id="rId9" xr:uid="{1B46049E-7FDB-4FF6-9A43-9D39D8123B23}"/>
+    <hyperlink ref="E2" r:id="rId10" xr:uid="{7F2186DB-5F0A-478D-8ABA-18A632F4AFA9}"/>
+    <hyperlink ref="D2" r:id="rId11" xr:uid="{36AA91A0-C9BC-4B14-A2ED-34EDE64D808F}"/>
+    <hyperlink ref="E10" r:id="rId12" xr:uid="{8DCB265B-8E3C-4980-ABC7-8A6393434105}"/>
+    <hyperlink ref="D10" r:id="rId13" xr:uid="{7EFE02F7-EA53-438F-8D7B-1EE7A8F2ACCF}"/>
+    <hyperlink ref="E11" r:id="rId14" xr:uid="{B7C41ED0-0748-466D-A777-87C0221011B3}"/>
+    <hyperlink ref="D11" r:id="rId15" xr:uid="{CDE1DE1F-C04F-4955-8CA7-40DDCE2A7869}"/>
+    <hyperlink ref="E6" r:id="rId16" xr:uid="{7CED1F56-7CEE-4740-AE25-A1F5ACD1F0BA}"/>
+    <hyperlink ref="D6" r:id="rId17" xr:uid="{41FE42E3-3745-4DB9-BAF7-CCAA19F6AE02}"/>
+    <hyperlink ref="E3" r:id="rId18" xr:uid="{2834821C-30B7-4BAB-A1CF-5FA292E134C3}"/>
+    <hyperlink ref="D3" r:id="rId19" xr:uid="{8D635CA0-58C6-4BAC-ADD8-803599AD66DE}"/>
+    <hyperlink ref="D12" r:id="rId20" xr:uid="{F7E95135-2938-42E0-8AF7-CA6E5A4EFEF3}"/>
+    <hyperlink ref="D5" r:id="rId21" xr:uid="{6DB4D0C8-8136-4767-8BB6-9EAFDDDC6960}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added components to file
</commit_message>
<xml_diff>
--- a/api/src/Service/resources/components.xlsx
+++ b/api/src/Service/resources/components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22920"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\environment-component\api\src\Service\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{453A2257-740E-4BFB-B941-CED8A88F8175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01162729-3A0F-4EC7-93D0-C92EFE74F196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="177">
   <si>
     <t>The environment excel file</t>
   </si>
@@ -519,6 +519,54 @@
   </si>
   <si>
     <t>https://github.com/ConductionNL/docparser/api/helm</t>
+  </si>
+  <si>
+    <t>qc</t>
+  </si>
+  <si>
+    <t>QueueComponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/Queue-Component/</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/Queue-Component/api/helm</t>
+  </si>
+  <si>
+    <t>brc</t>
+  </si>
+  <si>
+    <t>BesmettingRegistratieComponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/besmettingregistratiecomponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/besmettingregistratiecomponent/api/helm</t>
+  </si>
+  <si>
+    <t>cgrc</t>
+  </si>
+  <si>
+    <t>CommongroundRegistratieComponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/Commongroundregistratiecomponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/Commongroundregistratiecomponent/api/helm</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>ProtoComponentCommonground</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/Proto-component-commonground</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/Proto-component-commonground/api/helm</t>
   </si>
 </sst>
 </file>
@@ -1322,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0233B350-72AF-4D84-A15D-5E384E813B54}">
-  <dimension ref="A1:XFD28"/>
+  <dimension ref="A1:XFD32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1789,6 +1837,62 @@
       </c>
       <c r="E28" s="1" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7 16384:16384">
+      <c r="A29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7 16384:16384">
+      <c r="A30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7 16384:16384">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7 16384:16384">
+      <c r="A32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1850,8 +1954,16 @@
     <hyperlink ref="E27" r:id="rId51" xr:uid="{58C9101D-1169-4B29-A720-1C0468798C61}"/>
     <hyperlink ref="D28" r:id="rId52" xr:uid="{EDB2932F-EB16-4707-9BB1-6D000FDA27A9}"/>
     <hyperlink ref="E28" r:id="rId53" xr:uid="{7FA01D52-0946-4135-9E98-95D310018431}"/>
+    <hyperlink ref="D29" r:id="rId54" xr:uid="{ED073684-494C-40F0-B4EE-55A55EEAF86B}"/>
+    <hyperlink ref="E29" r:id="rId55" xr:uid="{11399521-E97B-41CD-BDC3-0119992A6EAB}"/>
+    <hyperlink ref="D30" r:id="rId56" xr:uid="{A438D0EE-A341-4A59-B446-0309BB1AAD47}"/>
+    <hyperlink ref="E30" r:id="rId57" xr:uid="{77762666-D702-49BD-A2AC-6D5CDE88A0B8}"/>
+    <hyperlink ref="D31" r:id="rId58" xr:uid="{B1B69E59-597E-48D1-A920-0F63BEF47DD0}"/>
+    <hyperlink ref="E31" r:id="rId59" xr:uid="{EB20FB1D-7AC1-4F98-84F3-2AF16FA04853}"/>
+    <hyperlink ref="D32" r:id="rId60" xr:uid="{47145844-13E9-4FA3-84DD-D32E98A04DCF}"/>
+    <hyperlink ref="E32" r:id="rId61" xr:uid="{96A8E6EF-06D5-4BF3-9804-D6A43B523CF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
</xml_diff>